<commit_message>
Updated all accuracies (final)
</commit_message>
<xml_diff>
--- a/Accuracy rMAE and rRMSE (Cross-Temporal).xlsx
+++ b/Accuracy rMAE and rRMSE (Cross-Temporal).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e00c848d2da39f20/Documents/3. Masters/Research/WindPowerForecasting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="565" documentId="8_{7CAE70F8-1326-4B7D-8A8A-809CD0BBBC40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53BD83A5-95DE-4191-9E10-1893C0F60EBC}"/>
+  <xr:revisionPtr revIDLastSave="566" documentId="8_{7CAE70F8-1326-4B7D-8A8A-809CD0BBBC40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77DBCF26-7BD2-4BA9-A05F-90D241A147B4}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{4F6B620E-8A72-45CF-9D17-FD2A4C076D11}"/>
+    <workbookView xWindow="15900" yWindow="0" windowWidth="22610" windowHeight="15370" xr2:uid="{4F6B620E-8A72-45CF-9D17-FD2A4C076D11}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -169,22 +169,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -200,6 +195,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -499,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9C5127F-CD46-4E4E-96B7-010FB4E47685}">
-  <dimension ref="A1:AI112"/>
+  <dimension ref="A1:AG112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="O40" sqref="O40"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="D110" sqref="D110:G110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -522,7 +521,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -541,7 +540,7 @@
       <c r="L1" s="2"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="4"/>
+      <c r="A2" s="5"/>
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
@@ -554,7 +553,7 @@
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3" s="4"/>
+      <c r="A3" s="5"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2">
         <v>2</v>
@@ -582,7 +581,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4" s="4"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
@@ -623,7 +622,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5" s="4"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="1"/>
       <c r="C5" s="2" t="s">
         <v>1</v>
@@ -660,7 +659,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A6" s="4"/>
+      <c r="A6" s="5"/>
       <c r="B6" s="1"/>
       <c r="C6" s="2" t="s">
         <v>2</v>
@@ -697,7 +696,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="4"/>
+      <c r="A7" s="5"/>
       <c r="B7" s="1"/>
       <c r="C7" s="2" t="s">
         <v>3</v>
@@ -774,7 +773,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -793,7 +792,7 @@
       <c r="L9" s="2"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" s="4"/>
+      <c r="A10" s="5"/>
       <c r="D10" s="1" t="s">
         <v>4</v>
       </c>
@@ -806,7 +805,7 @@
       <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A11" s="4"/>
+      <c r="A11" s="5"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2">
         <v>2</v>
@@ -834,7 +833,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A12" s="4"/>
+      <c r="A12" s="5"/>
       <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
@@ -875,7 +874,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A13" s="4"/>
+      <c r="A13" s="5"/>
       <c r="B13" s="1"/>
       <c r="C13" s="2" t="s">
         <v>1</v>
@@ -912,7 +911,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A14" s="4"/>
+      <c r="A14" s="5"/>
       <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
         <v>2</v>
@@ -949,7 +948,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A15" s="4"/>
+      <c r="A15" s="5"/>
       <c r="B15" s="1"/>
       <c r="C15" s="2" t="s">
         <v>3</v>
@@ -1025,8 +1024,8 @@
         <v>0.57856822969324828</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A17" s="4" t="s">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1044,8 +1043,8 @@
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A18" s="4"/>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A18" s="5"/>
       <c r="D18" s="1" t="s">
         <v>4</v>
       </c>
@@ -1057,8 +1056,8 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A19" s="4"/>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A19" s="5"/>
       <c r="D19" s="2">
         <v>2</v>
       </c>
@@ -1084,8 +1083,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A20" s="4"/>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A20" s="5"/>
       <c r="B20" s="1" t="s">
         <v>5</v>
       </c>
@@ -1125,8 +1124,8 @@
         <v>1.0941536533282454</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A21" s="4"/>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A21" s="5"/>
       <c r="B21" s="1"/>
       <c r="C21" s="2" t="s">
         <v>1</v>
@@ -1162,8 +1161,8 @@
         <v>0.69377176654106154</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A22" s="4"/>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A22" s="5"/>
       <c r="B22" s="1"/>
       <c r="C22" s="2" t="s">
         <v>2</v>
@@ -1199,8 +1198,8 @@
         <v>0.53584339752284194</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A23" s="4"/>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A23" s="5"/>
       <c r="B23" s="1"/>
       <c r="C23" s="2" t="s">
         <v>3</v>
@@ -1236,7 +1235,7 @@
         <v>0.30534989621986136</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.35">
       <c r="C24" s="2" t="s">
         <v>16</v>
       </c>
@@ -1275,27 +1274,9 @@
         <f>GEOMEAN(M20:M23)</f>
         <v>0.59365297608650891</v>
       </c>
-      <c r="R24" s="5"/>
-      <c r="S24" s="5"/>
-      <c r="T24" s="5"/>
-      <c r="U24" s="5"/>
-      <c r="V24" s="5"/>
-      <c r="W24" s="5"/>
-      <c r="X24" s="5"/>
-      <c r="Y24" s="5"/>
-      <c r="Z24" s="5"/>
-      <c r="AA24" s="5"/>
-      <c r="AB24" s="5"/>
-      <c r="AC24" s="5"/>
-      <c r="AD24" s="5"/>
-      <c r="AE24" s="5"/>
-      <c r="AF24" s="5"/>
-      <c r="AG24" s="5"/>
-      <c r="AH24" s="5"/>
-      <c r="AI24" s="5"/>
-    </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A25" s="4" t="s">
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A25" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1312,27 +1293,9 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
-      <c r="R25" s="5"/>
-      <c r="S25" s="5"/>
-      <c r="T25" s="5"/>
-      <c r="U25" s="5"/>
-      <c r="V25" s="5"/>
-      <c r="W25" s="5"/>
-      <c r="X25" s="5"/>
-      <c r="Y25" s="5"/>
-      <c r="Z25" s="5"/>
-      <c r="AA25" s="5"/>
-      <c r="AB25" s="5"/>
-      <c r="AC25" s="5"/>
-      <c r="AD25" s="5"/>
-      <c r="AE25" s="5"/>
-      <c r="AF25" s="5"/>
-      <c r="AG25" s="5"/>
-      <c r="AH25" s="5"/>
-      <c r="AI25" s="5"/>
-    </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A26" s="4"/>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A26" s="5"/>
       <c r="D26" s="1" t="s">
         <v>4</v>
       </c>
@@ -1343,27 +1306,9 @@
       </c>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
-      <c r="R26" s="5"/>
-      <c r="S26" s="5"/>
-      <c r="T26" s="5"/>
-      <c r="U26" s="5"/>
-      <c r="V26" s="5"/>
-      <c r="W26" s="5"/>
-      <c r="X26" s="5"/>
-      <c r="Y26" s="5"/>
-      <c r="Z26" s="5"/>
-      <c r="AA26" s="5"/>
-      <c r="AB26" s="5"/>
-      <c r="AC26" s="5"/>
-      <c r="AD26" s="5"/>
-      <c r="AE26" s="5"/>
-      <c r="AF26" s="5"/>
-      <c r="AG26" s="5"/>
-      <c r="AH26" s="5"/>
-      <c r="AI26" s="5"/>
-    </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A27" s="4"/>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A27" s="5"/>
       <c r="D27" s="2">
         <v>2</v>
       </c>
@@ -1388,27 +1333,9 @@
       <c r="M27" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R27" s="5"/>
-      <c r="S27" s="5"/>
-      <c r="T27" s="5"/>
-      <c r="U27" s="5"/>
-      <c r="V27" s="5"/>
-      <c r="W27" s="5"/>
-      <c r="X27" s="5"/>
-      <c r="Y27" s="5"/>
-      <c r="Z27" s="5"/>
-      <c r="AA27" s="5"/>
-      <c r="AB27" s="5"/>
-      <c r="AC27" s="5"/>
-      <c r="AD27" s="5"/>
-      <c r="AE27" s="5"/>
-      <c r="AF27" s="5"/>
-      <c r="AG27" s="5"/>
-      <c r="AH27" s="5"/>
-      <c r="AI27" s="5"/>
-    </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A28" s="4"/>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A28" s="5"/>
       <c r="B28" s="1" t="s">
         <v>5</v>
       </c>
@@ -1447,27 +1374,9 @@
         <f>GEOMEAN(J28:L28)</f>
         <v>1.0888325421285385</v>
       </c>
-      <c r="R28" s="5"/>
-      <c r="S28" s="5"/>
-      <c r="T28" s="5"/>
-      <c r="U28" s="5"/>
-      <c r="V28" s="5"/>
-      <c r="W28" s="5"/>
-      <c r="X28" s="5"/>
-      <c r="Y28" s="5"/>
-      <c r="Z28" s="5"/>
-      <c r="AA28" s="5"/>
-      <c r="AB28" s="5"/>
-      <c r="AC28" s="5"/>
-      <c r="AD28" s="5"/>
-      <c r="AE28" s="5"/>
-      <c r="AF28" s="5"/>
-      <c r="AG28" s="5"/>
-      <c r="AH28" s="5"/>
-      <c r="AI28" s="5"/>
-    </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A29" s="4"/>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A29" s="5"/>
       <c r="B29" s="1"/>
       <c r="C29" s="2" t="s">
         <v>1</v>
@@ -1502,27 +1411,9 @@
         <f>GEOMEAN(J29:L29)</f>
         <v>0.68771564685504094</v>
       </c>
-      <c r="R29" s="5"/>
-      <c r="S29" s="5"/>
-      <c r="T29" s="5"/>
-      <c r="U29" s="5"/>
-      <c r="V29" s="5"/>
-      <c r="W29" s="5"/>
-      <c r="X29" s="5"/>
-      <c r="Y29" s="5"/>
-      <c r="Z29" s="5"/>
-      <c r="AA29" s="5"/>
-      <c r="AB29" s="5"/>
-      <c r="AC29" s="5"/>
-      <c r="AD29" s="5"/>
-      <c r="AE29" s="5"/>
-      <c r="AF29" s="5"/>
-      <c r="AG29" s="5"/>
-      <c r="AH29" s="5"/>
-      <c r="AI29" s="5"/>
-    </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A30" s="4"/>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A30" s="5"/>
       <c r="B30" s="1"/>
       <c r="C30" s="2" t="s">
         <v>2</v>
@@ -1557,27 +1448,19 @@
         <f>GEOMEAN(J30:L30)</f>
         <v>0.53029052178649372</v>
       </c>
-      <c r="R30" s="5"/>
-      <c r="S30" s="5"/>
-      <c r="T30" s="5"/>
-      <c r="U30" s="5"/>
-      <c r="V30" s="6"/>
-      <c r="W30" s="6"/>
-      <c r="X30" s="6"/>
-      <c r="Y30" s="6"/>
-      <c r="Z30" s="6"/>
-      <c r="AA30" s="5"/>
-      <c r="AB30" s="6"/>
-      <c r="AC30" s="6"/>
-      <c r="AD30" s="6"/>
-      <c r="AE30" s="6"/>
-      <c r="AF30" s="6"/>
-      <c r="AG30" s="5"/>
-      <c r="AH30" s="5"/>
-      <c r="AI30" s="5"/>
-    </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A31" s="4"/>
+      <c r="V30" s="2"/>
+      <c r="W30" s="2"/>
+      <c r="X30" s="2"/>
+      <c r="Y30" s="2"/>
+      <c r="Z30" s="2"/>
+      <c r="AB30" s="2"/>
+      <c r="AC30" s="2"/>
+      <c r="AD30" s="2"/>
+      <c r="AE30" s="2"/>
+      <c r="AF30" s="2"/>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A31" s="5"/>
       <c r="B31" s="1"/>
       <c r="C31" s="2" t="s">
         <v>3</v>
@@ -1612,26 +1495,14 @@
         <f>GEOMEAN(J31:L31)</f>
         <v>0.29643269094669394</v>
       </c>
-      <c r="R31" s="5"/>
-      <c r="S31" s="5"/>
-      <c r="T31" s="5"/>
-      <c r="U31" s="5"/>
-      <c r="V31" s="5"/>
-      <c r="W31" s="5"/>
-      <c r="X31" s="7"/>
-      <c r="Y31" s="7"/>
-      <c r="Z31" s="7"/>
-      <c r="AA31" s="5"/>
-      <c r="AB31" s="5"/>
-      <c r="AC31" s="5"/>
-      <c r="AD31" s="7"/>
-      <c r="AE31" s="7"/>
-      <c r="AF31" s="7"/>
-      <c r="AG31" s="5"/>
-      <c r="AH31" s="5"/>
-      <c r="AI31" s="5"/>
-    </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1"/>
+      <c r="Z31" s="1"/>
+      <c r="AD31" s="1"/>
+      <c r="AE31" s="1"/>
+      <c r="AF31" s="1"/>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.35">
       <c r="C32" s="2" t="s">
         <v>16</v>
       </c>
@@ -1670,27 +1541,18 @@
         <f>GEOMEAN(M28:M31)</f>
         <v>0.58573677234427501</v>
       </c>
-      <c r="R32" s="5"/>
-      <c r="S32" s="5"/>
-      <c r="T32" s="5"/>
-      <c r="U32" s="5"/>
-      <c r="V32" s="5"/>
-      <c r="W32" s="6"/>
-      <c r="X32" s="6"/>
-      <c r="Y32" s="6"/>
-      <c r="Z32" s="6"/>
-      <c r="AA32" s="6"/>
-      <c r="AB32" s="5"/>
-      <c r="AC32" s="5"/>
-      <c r="AD32" s="6"/>
-      <c r="AE32" s="6"/>
-      <c r="AF32" s="6"/>
-      <c r="AG32" s="6"/>
-      <c r="AH32" s="5"/>
-      <c r="AI32" s="5"/>
-    </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A33" s="4" t="s">
+      <c r="W32" s="2"/>
+      <c r="X32" s="2"/>
+      <c r="Y32" s="2"/>
+      <c r="Z32" s="2"/>
+      <c r="AA32" s="2"/>
+      <c r="AD32" s="2"/>
+      <c r="AE32" s="2"/>
+      <c r="AF32" s="2"/>
+      <c r="AG32" s="2"/>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A33" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -1707,27 +1569,21 @@
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
-      <c r="R33" s="5"/>
-      <c r="S33" s="5"/>
-      <c r="T33" s="5"/>
-      <c r="U33" s="5"/>
-      <c r="V33" s="7"/>
-      <c r="W33" s="6"/>
-      <c r="X33" s="8"/>
-      <c r="Y33" s="8"/>
-      <c r="Z33" s="8"/>
-      <c r="AA33" s="8"/>
-      <c r="AB33" s="7"/>
-      <c r="AC33" s="6"/>
-      <c r="AD33" s="8"/>
-      <c r="AE33" s="8"/>
-      <c r="AF33" s="8"/>
-      <c r="AG33" s="8"/>
-      <c r="AH33" s="5"/>
-      <c r="AI33" s="5"/>
-    </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A34" s="4"/>
+      <c r="V33" s="1"/>
+      <c r="W33" s="2"/>
+      <c r="X33" s="4"/>
+      <c r="Y33" s="4"/>
+      <c r="Z33" s="4"/>
+      <c r="AA33" s="4"/>
+      <c r="AB33" s="1"/>
+      <c r="AC33" s="2"/>
+      <c r="AD33" s="4"/>
+      <c r="AE33" s="4"/>
+      <c r="AF33" s="4"/>
+      <c r="AG33" s="4"/>
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A34" s="5"/>
       <c r="D34" s="1" t="s">
         <v>4</v>
       </c>
@@ -1738,27 +1594,21 @@
       </c>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
-      <c r="R34" s="5"/>
-      <c r="S34" s="5"/>
-      <c r="T34" s="5"/>
-      <c r="U34" s="5"/>
-      <c r="V34" s="7"/>
-      <c r="W34" s="6"/>
-      <c r="X34" s="8"/>
-      <c r="Y34" s="8"/>
-      <c r="Z34" s="8"/>
-      <c r="AA34" s="8"/>
-      <c r="AB34" s="7"/>
-      <c r="AC34" s="6"/>
-      <c r="AD34" s="8"/>
-      <c r="AE34" s="8"/>
-      <c r="AF34" s="8"/>
-      <c r="AG34" s="8"/>
-      <c r="AH34" s="5"/>
-      <c r="AI34" s="5"/>
-    </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A35" s="4"/>
+      <c r="V34" s="1"/>
+      <c r="W34" s="2"/>
+      <c r="X34" s="4"/>
+      <c r="Y34" s="4"/>
+      <c r="Z34" s="4"/>
+      <c r="AA34" s="4"/>
+      <c r="AB34" s="1"/>
+      <c r="AC34" s="2"/>
+      <c r="AD34" s="4"/>
+      <c r="AE34" s="4"/>
+      <c r="AF34" s="4"/>
+      <c r="AG34" s="4"/>
+    </row>
+    <row r="35" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A35" s="5"/>
       <c r="D35" s="2">
         <v>2</v>
       </c>
@@ -1783,27 +1633,21 @@
       <c r="M35" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R35" s="5"/>
-      <c r="S35" s="5"/>
-      <c r="T35" s="5"/>
-      <c r="U35" s="5"/>
-      <c r="V35" s="7"/>
-      <c r="W35" s="6"/>
-      <c r="X35" s="8"/>
-      <c r="Y35" s="8"/>
-      <c r="Z35" s="8"/>
-      <c r="AA35" s="8"/>
-      <c r="AB35" s="7"/>
-      <c r="AC35" s="6"/>
-      <c r="AD35" s="8"/>
-      <c r="AE35" s="8"/>
-      <c r="AF35" s="8"/>
-      <c r="AG35" s="8"/>
-      <c r="AH35" s="5"/>
-      <c r="AI35" s="5"/>
-    </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A36" s="4"/>
+      <c r="V35" s="1"/>
+      <c r="W35" s="2"/>
+      <c r="X35" s="4"/>
+      <c r="Y35" s="4"/>
+      <c r="Z35" s="4"/>
+      <c r="AA35" s="4"/>
+      <c r="AB35" s="1"/>
+      <c r="AC35" s="2"/>
+      <c r="AD35" s="4"/>
+      <c r="AE35" s="4"/>
+      <c r="AF35" s="4"/>
+      <c r="AG35" s="4"/>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A36" s="5"/>
       <c r="B36" s="1" t="s">
         <v>5</v>
       </c>
@@ -1842,27 +1686,21 @@
         <f>GEOMEAN(J36:L36)</f>
         <v>1.1001948253851705</v>
       </c>
-      <c r="R36" s="5"/>
-      <c r="S36" s="5"/>
-      <c r="T36" s="5"/>
-      <c r="U36" s="5"/>
-      <c r="V36" s="7"/>
-      <c r="W36" s="6"/>
-      <c r="X36" s="8"/>
-      <c r="Y36" s="8"/>
-      <c r="Z36" s="8"/>
-      <c r="AA36" s="8"/>
-      <c r="AB36" s="7"/>
-      <c r="AC36" s="6"/>
-      <c r="AD36" s="8"/>
-      <c r="AE36" s="8"/>
-      <c r="AF36" s="8"/>
-      <c r="AG36" s="8"/>
-      <c r="AH36" s="5"/>
-      <c r="AI36" s="5"/>
-    </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A37" s="4"/>
+      <c r="V36" s="1"/>
+      <c r="W36" s="2"/>
+      <c r="X36" s="4"/>
+      <c r="Y36" s="4"/>
+      <c r="Z36" s="4"/>
+      <c r="AA36" s="4"/>
+      <c r="AB36" s="1"/>
+      <c r="AC36" s="2"/>
+      <c r="AD36" s="4"/>
+      <c r="AE36" s="4"/>
+      <c r="AF36" s="4"/>
+      <c r="AG36" s="4"/>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A37" s="5"/>
       <c r="B37" s="1"/>
       <c r="C37" s="2" t="s">
         <v>1</v>
@@ -1897,27 +1735,19 @@
         <f>GEOMEAN(J37:L37)</f>
         <v>0.69611358888790298</v>
       </c>
-      <c r="R37" s="5"/>
-      <c r="S37" s="5"/>
-      <c r="T37" s="5"/>
-      <c r="U37" s="5"/>
-      <c r="V37" s="5"/>
-      <c r="W37" s="6"/>
-      <c r="X37" s="8"/>
-      <c r="Y37" s="8"/>
-      <c r="Z37" s="8"/>
-      <c r="AA37" s="8"/>
-      <c r="AB37" s="5"/>
-      <c r="AC37" s="6"/>
-      <c r="AD37" s="8"/>
-      <c r="AE37" s="8"/>
-      <c r="AF37" s="8"/>
-      <c r="AG37" s="8"/>
-      <c r="AH37" s="5"/>
-      <c r="AI37" s="5"/>
-    </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A38" s="4"/>
+      <c r="W37" s="2"/>
+      <c r="X37" s="4"/>
+      <c r="Y37" s="4"/>
+      <c r="Z37" s="4"/>
+      <c r="AA37" s="4"/>
+      <c r="AC37" s="2"/>
+      <c r="AD37" s="4"/>
+      <c r="AE37" s="4"/>
+      <c r="AF37" s="4"/>
+      <c r="AG37" s="4"/>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A38" s="5"/>
       <c r="B38" s="1"/>
       <c r="C38" s="2" t="s">
         <v>2</v>
@@ -1952,27 +1782,9 @@
         <f>GEOMEAN(J38:L38)</f>
         <v>0.53765982147751423</v>
       </c>
-      <c r="R38" s="5"/>
-      <c r="S38" s="5"/>
-      <c r="T38" s="5"/>
-      <c r="U38" s="5"/>
-      <c r="V38" s="5"/>
-      <c r="W38" s="5"/>
-      <c r="X38" s="5"/>
-      <c r="Y38" s="5"/>
-      <c r="Z38" s="5"/>
-      <c r="AA38" s="5"/>
-      <c r="AB38" s="5"/>
-      <c r="AC38" s="5"/>
-      <c r="AD38" s="5"/>
-      <c r="AE38" s="5"/>
-      <c r="AF38" s="5"/>
-      <c r="AG38" s="5"/>
-      <c r="AH38" s="5"/>
-      <c r="AI38" s="5"/>
-    </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A39" s="4"/>
+    </row>
+    <row r="39" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A39" s="5"/>
       <c r="B39" s="1"/>
       <c r="C39" s="2" t="s">
         <v>3</v>
@@ -2007,26 +1819,8 @@
         <f>GEOMEAN(J39:L39)</f>
         <v>0.30412609066719809</v>
       </c>
-      <c r="R39" s="5"/>
-      <c r="S39" s="5"/>
-      <c r="T39" s="5"/>
-      <c r="U39" s="5"/>
-      <c r="V39" s="5"/>
-      <c r="W39" s="5"/>
-      <c r="X39" s="5"/>
-      <c r="Y39" s="5"/>
-      <c r="Z39" s="5"/>
-      <c r="AA39" s="5"/>
-      <c r="AB39" s="5"/>
-      <c r="AC39" s="5"/>
-      <c r="AD39" s="5"/>
-      <c r="AE39" s="5"/>
-      <c r="AF39" s="5"/>
-      <c r="AG39" s="5"/>
-      <c r="AH39" s="5"/>
-      <c r="AI39" s="5"/>
-    </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.35">
       <c r="C40" s="2" t="s">
         <v>16</v>
       </c>
@@ -2065,27 +1859,9 @@
         <f>GEOMEAN(M36:M39)</f>
         <v>0.59487777423582822</v>
       </c>
-      <c r="R40" s="5"/>
-      <c r="S40" s="5"/>
-      <c r="T40" s="5"/>
-      <c r="U40" s="5"/>
-      <c r="V40" s="5"/>
-      <c r="W40" s="5"/>
-      <c r="X40" s="5"/>
-      <c r="Y40" s="5"/>
-      <c r="Z40" s="5"/>
-      <c r="AA40" s="5"/>
-      <c r="AB40" s="5"/>
-      <c r="AC40" s="5"/>
-      <c r="AD40" s="5"/>
-      <c r="AE40" s="5"/>
-      <c r="AF40" s="5"/>
-      <c r="AG40" s="5"/>
-      <c r="AH40" s="5"/>
-      <c r="AI40" s="5"/>
-    </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A41" s="4" t="s">
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A41" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -2102,27 +1878,9 @@
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
-      <c r="R41" s="5"/>
-      <c r="S41" s="5"/>
-      <c r="T41" s="5"/>
-      <c r="U41" s="5"/>
-      <c r="V41" s="5"/>
-      <c r="W41" s="5"/>
-      <c r="X41" s="5"/>
-      <c r="Y41" s="5"/>
-      <c r="Z41" s="5"/>
-      <c r="AA41" s="5"/>
-      <c r="AB41" s="5"/>
-      <c r="AC41" s="5"/>
-      <c r="AD41" s="5"/>
-      <c r="AE41" s="5"/>
-      <c r="AF41" s="5"/>
-      <c r="AG41" s="5"/>
-      <c r="AH41" s="5"/>
-      <c r="AI41" s="5"/>
-    </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A42" s="4"/>
+    </row>
+    <row r="42" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A42" s="5"/>
       <c r="D42" s="1" t="s">
         <v>4</v>
       </c>
@@ -2133,27 +1891,9 @@
       </c>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
-      <c r="R42" s="5"/>
-      <c r="S42" s="5"/>
-      <c r="T42" s="5"/>
-      <c r="U42" s="5"/>
-      <c r="V42" s="5"/>
-      <c r="W42" s="5"/>
-      <c r="X42" s="5"/>
-      <c r="Y42" s="5"/>
-      <c r="Z42" s="5"/>
-      <c r="AA42" s="5"/>
-      <c r="AB42" s="5"/>
-      <c r="AC42" s="5"/>
-      <c r="AD42" s="5"/>
-      <c r="AE42" s="5"/>
-      <c r="AF42" s="5"/>
-      <c r="AG42" s="5"/>
-      <c r="AH42" s="5"/>
-      <c r="AI42" s="5"/>
-    </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A43" s="4"/>
+    </row>
+    <row r="43" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A43" s="5"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2">
         <v>2</v>
@@ -2180,8 +1920,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A44" s="4"/>
+    <row r="44" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A44" s="5"/>
       <c r="B44" s="1" t="s">
         <v>5</v>
       </c>
@@ -2221,8 +1961,8 @@
         <v>1.0806715630344856</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A45" s="4"/>
+    <row r="45" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A45" s="5"/>
       <c r="B45" s="1"/>
       <c r="C45" s="2" t="s">
         <v>1</v>
@@ -2258,8 +1998,8 @@
         <v>0.67694612307450464</v>
       </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A46" s="4"/>
+    <row r="46" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A46" s="5"/>
       <c r="B46" s="1"/>
       <c r="C46" s="2" t="s">
         <v>2</v>
@@ -2295,8 +2035,8 @@
         <v>0.52080950490338696</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A47" s="4"/>
+    <row r="47" spans="1:33" x14ac:dyDescent="0.35">
+      <c r="A47" s="5"/>
       <c r="B47" s="1"/>
       <c r="C47" s="2" t="s">
         <v>3</v>
@@ -2332,7 +2072,7 @@
         <v>0.29039297925087221</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.35">
       <c r="C48" s="2" t="s">
         <v>16</v>
       </c>
@@ -2373,7 +2113,7 @@
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A49" s="4" t="s">
+      <c r="A49" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B49" s="2" t="s">
@@ -2392,7 +2132,7 @@
       <c r="L49" s="2"/>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A50" s="4"/>
+      <c r="A50" s="5"/>
       <c r="D50" s="1" t="s">
         <v>4</v>
       </c>
@@ -2405,7 +2145,7 @@
       <c r="L50" s="1"/>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A51" s="4"/>
+      <c r="A51" s="5"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2">
         <v>2</v>
@@ -2433,7 +2173,7 @@
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A52" s="4"/>
+      <c r="A52" s="5"/>
       <c r="B52" s="1" t="s">
         <v>5</v>
       </c>
@@ -2474,7 +2214,7 @@
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A53" s="4"/>
+      <c r="A53" s="5"/>
       <c r="B53" s="1"/>
       <c r="C53" s="2" t="s">
         <v>1</v>
@@ -2511,7 +2251,7 @@
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A54" s="4"/>
+      <c r="A54" s="5"/>
       <c r="B54" s="1"/>
       <c r="C54" s="2" t="s">
         <v>2</v>
@@ -2548,7 +2288,7 @@
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A55" s="4"/>
+      <c r="A55" s="5"/>
       <c r="B55" s="1"/>
       <c r="C55" s="2" t="s">
         <v>3</v>
@@ -2625,7 +2365,7 @@
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B57" s="2" t="s">
@@ -2644,7 +2384,7 @@
       <c r="L57" s="2"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A58" s="4"/>
+      <c r="A58" s="5"/>
       <c r="D58" s="1" t="s">
         <v>4</v>
       </c>
@@ -2657,7 +2397,7 @@
       <c r="L58" s="1"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A59" s="4"/>
+      <c r="A59" s="5"/>
       <c r="D59">
         <v>2</v>
       </c>
@@ -2684,7 +2424,7 @@
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A60" s="4"/>
+      <c r="A60" s="5"/>
       <c r="B60" s="1" t="s">
         <v>5</v>
       </c>
@@ -2725,7 +2465,7 @@
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A61" s="4"/>
+      <c r="A61" s="5"/>
       <c r="B61" s="1"/>
       <c r="C61" t="s">
         <v>1</v>
@@ -2762,7 +2502,7 @@
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A62" s="4"/>
+      <c r="A62" s="5"/>
       <c r="B62" s="1"/>
       <c r="C62" t="s">
         <v>2</v>
@@ -2799,7 +2539,7 @@
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A63" s="4"/>
+      <c r="A63" s="5"/>
       <c r="B63" s="1"/>
       <c r="C63" t="s">
         <v>3</v>
@@ -2876,7 +2616,7 @@
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A65" s="4" t="s">
+      <c r="A65" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B65" s="2" t="s">
@@ -2895,7 +2635,7 @@
       <c r="L65" s="2"/>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A66" s="4"/>
+      <c r="A66" s="5"/>
       <c r="D66" s="1" t="s">
         <v>4</v>
       </c>
@@ -2908,7 +2648,7 @@
       <c r="L66" s="1"/>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A67" s="4"/>
+      <c r="A67" s="5"/>
       <c r="D67">
         <v>2</v>
       </c>
@@ -2929,7 +2669,7 @@
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A68" s="4"/>
+      <c r="A68" s="5"/>
       <c r="B68" s="1" t="s">
         <v>5</v>
       </c>
@@ -2970,7 +2710,7 @@
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A69" s="4"/>
+      <c r="A69" s="5"/>
       <c r="B69" s="1"/>
       <c r="C69" t="s">
         <v>1</v>
@@ -3007,7 +2747,7 @@
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A70" s="4"/>
+      <c r="A70" s="5"/>
       <c r="B70" s="1"/>
       <c r="C70" t="s">
         <v>2</v>
@@ -3044,7 +2784,7 @@
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A71" s="4"/>
+      <c r="A71" s="5"/>
       <c r="B71" s="1"/>
       <c r="C71" t="s">
         <v>3</v>
@@ -3121,7 +2861,7 @@
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A73" s="4" t="s">
+      <c r="A73" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B73" s="2" t="s">
@@ -3140,7 +2880,7 @@
       <c r="L73" s="2"/>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A74" s="4"/>
+      <c r="A74" s="5"/>
       <c r="D74" s="1" t="s">
         <v>4</v>
       </c>
@@ -3153,7 +2893,7 @@
       <c r="L74" s="1"/>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A75" s="4"/>
+      <c r="A75" s="5"/>
       <c r="D75">
         <v>2</v>
       </c>
@@ -3174,7 +2914,7 @@
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A76" s="4"/>
+      <c r="A76" s="5"/>
       <c r="B76" s="1" t="s">
         <v>5</v>
       </c>
@@ -3215,7 +2955,7 @@
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A77" s="4"/>
+      <c r="A77" s="5"/>
       <c r="B77" s="1"/>
       <c r="C77" t="s">
         <v>1</v>
@@ -3252,7 +2992,7 @@
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A78" s="4"/>
+      <c r="A78" s="5"/>
       <c r="B78" s="1"/>
       <c r="C78" t="s">
         <v>2</v>
@@ -3289,7 +3029,7 @@
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A79" s="4"/>
+      <c r="A79" s="5"/>
       <c r="B79" s="1"/>
       <c r="C79" t="s">
         <v>3</v>
@@ -3366,7 +3106,7 @@
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A81" s="4" t="s">
+      <c r="A81" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B81" s="2" t="s">
@@ -3385,7 +3125,7 @@
       <c r="L81" s="2"/>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A82" s="4"/>
+      <c r="A82" s="5"/>
       <c r="D82" s="1" t="s">
         <v>4</v>
       </c>
@@ -3398,7 +3138,7 @@
       <c r="L82" s="1"/>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A83" s="4"/>
+      <c r="A83" s="5"/>
       <c r="D83">
         <v>2</v>
       </c>
@@ -3419,7 +3159,7 @@
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A84" s="4"/>
+      <c r="A84" s="5"/>
       <c r="B84" s="1" t="s">
         <v>5</v>
       </c>
@@ -3460,7 +3200,7 @@
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A85" s="4"/>
+      <c r="A85" s="5"/>
       <c r="B85" s="1"/>
       <c r="C85" t="s">
         <v>1</v>
@@ -3497,7 +3237,7 @@
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A86" s="4"/>
+      <c r="A86" s="5"/>
       <c r="B86" s="1"/>
       <c r="C86" t="s">
         <v>2</v>
@@ -3534,7 +3274,7 @@
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A87" s="4"/>
+      <c r="A87" s="5"/>
       <c r="B87" s="1"/>
       <c r="C87" t="s">
         <v>3</v>
@@ -3611,7 +3351,7 @@
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A89" s="4" t="s">
+      <c r="A89" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B89" s="2" t="s">
@@ -3630,7 +3370,7 @@
       <c r="L89" s="2"/>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A90" s="4"/>
+      <c r="A90" s="5"/>
       <c r="D90" s="1" t="s">
         <v>4</v>
       </c>
@@ -3643,7 +3383,7 @@
       <c r="L90" s="1"/>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A91" s="4"/>
+      <c r="A91" s="5"/>
       <c r="D91">
         <v>2</v>
       </c>
@@ -3664,7 +3404,7 @@
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A92" s="4"/>
+      <c r="A92" s="5"/>
       <c r="B92" s="1" t="s">
         <v>5</v>
       </c>
@@ -3705,7 +3445,7 @@
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A93" s="4"/>
+      <c r="A93" s="5"/>
       <c r="B93" s="1"/>
       <c r="C93" t="s">
         <v>1</v>
@@ -3742,7 +3482,7 @@
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A94" s="4"/>
+      <c r="A94" s="5"/>
       <c r="B94" s="1"/>
       <c r="C94" t="s">
         <v>2</v>
@@ -3779,7 +3519,7 @@
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A95" s="4"/>
+      <c r="A95" s="5"/>
       <c r="B95" s="1"/>
       <c r="C95" t="s">
         <v>3</v>
@@ -3856,7 +3596,7 @@
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A97" s="4" t="s">
+      <c r="A97" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B97" s="2" t="s">
@@ -3875,7 +3615,7 @@
       <c r="L97" s="2"/>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A98" s="4"/>
+      <c r="A98" s="5"/>
       <c r="D98" s="1" t="s">
         <v>4</v>
       </c>
@@ -3888,7 +3628,7 @@
       <c r="L98" s="1"/>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A99" s="4"/>
+      <c r="A99" s="5"/>
       <c r="D99">
         <v>2</v>
       </c>
@@ -3909,7 +3649,7 @@
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A100" s="4"/>
+      <c r="A100" s="5"/>
       <c r="B100" s="1" t="s">
         <v>5</v>
       </c>
@@ -3950,7 +3690,7 @@
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A101" s="4"/>
+      <c r="A101" s="5"/>
       <c r="B101" s="1"/>
       <c r="C101" t="s">
         <v>1</v>
@@ -3987,7 +3727,7 @@
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A102" s="4"/>
+      <c r="A102" s="5"/>
       <c r="B102" s="1"/>
       <c r="C102" t="s">
         <v>2</v>
@@ -4024,7 +3764,7 @@
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A103" s="4"/>
+      <c r="A103" s="5"/>
       <c r="B103" s="1"/>
       <c r="C103" t="s">
         <v>3</v>
@@ -4101,7 +3841,7 @@
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A105" s="4" t="s">
+      <c r="A105" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B105" s="2" t="s">
@@ -4120,7 +3860,7 @@
       <c r="L105" s="2"/>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A106" s="4"/>
+      <c r="A106" s="5"/>
       <c r="D106" s="1" t="s">
         <v>4</v>
       </c>
@@ -4133,7 +3873,7 @@
       <c r="L106" s="1"/>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A107" s="4"/>
+      <c r="A107" s="5"/>
       <c r="D107">
         <v>2</v>
       </c>
@@ -4154,7 +3894,7 @@
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A108" s="4"/>
+      <c r="A108" s="5"/>
       <c r="B108" s="1" t="s">
         <v>5</v>
       </c>
@@ -4195,7 +3935,7 @@
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A109" s="4"/>
+      <c r="A109" s="5"/>
       <c r="B109" s="1"/>
       <c r="C109" t="s">
         <v>1</v>
@@ -4232,7 +3972,7 @@
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A110" s="4"/>
+      <c r="A110" s="5"/>
       <c r="B110" s="1"/>
       <c r="C110" t="s">
         <v>2</v>
@@ -4269,7 +4009,7 @@
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A111" s="4"/>
+      <c r="A111" s="5"/>
       <c r="B111" s="1"/>
       <c r="C111" t="s">
         <v>3</v>
@@ -4347,6 +4087,7 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A1:A7"/>
     <mergeCell ref="A105:A111"/>
     <mergeCell ref="A9:A15"/>
     <mergeCell ref="A17:A23"/>
@@ -4360,7 +4101,6 @@
     <mergeCell ref="A33:A39"/>
     <mergeCell ref="A41:A47"/>
     <mergeCell ref="A49:A55"/>
-    <mergeCell ref="A1:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>